<commit_message>
data till 14 Mar 8AM
</commit_message>
<xml_diff>
--- a/Inventory Order Book.xlsx
+++ b/Inventory Order Book.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815"/>
+    <workbookView windowWidth="19815" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SIM" sheetId="1" r:id="rId1"/>
+    <sheet name="Phone" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>S.No.</t>
   </si>
@@ -38,22 +39,60 @@
   </si>
   <si>
     <t>Connectivity</t>
+  </si>
+  <si>
+    <t>Fund transfered for phone</t>
+  </si>
+  <si>
+    <t>Transaction Id</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Cash from Magadh</t>
+  </si>
+  <si>
+    <t>AXIR210586970004</t>
+  </si>
+  <si>
+    <t>Net from Axis</t>
+  </si>
+  <si>
+    <t>AXIR210597327835</t>
+  </si>
+  <si>
+    <t>AXIR210607602459</t>
+  </si>
+  <si>
+    <t>AXIR210682362776</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -75,14 +114,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -96,6 +150,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -104,26 +182,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -136,7 +199,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,66 +222,27 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -218,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,193 +266,211 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,15 +481,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -447,6 +495,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -466,15 +523,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -486,26 +534,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,20 +552,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -547,144 +604,168 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1011,8 +1092,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1027,22 +1108,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1056,7 +1137,7 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="12">
         <v>44531</v>
       </c>
       <c r="E2" s="1">
@@ -1076,7 +1157,7 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="12">
         <v>44201</v>
       </c>
       <c r="E3" s="1">
@@ -1096,7 +1177,7 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="12">
         <v>44234</v>
       </c>
       <c r="E4" s="1">
@@ -1116,7 +1197,7 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="12">
         <v>44257</v>
       </c>
       <c r="E5" s="1">
@@ -1130,4 +1211,176 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="6.28571428571429" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85714285714286" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5714285714286" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.71428571428571" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.1428571428571" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.8571428571429" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.71428571428571" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.57142857142857" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.14285714285714" style="4" customWidth="1"/>
+    <col min="10" max="10" width="6.28571428571429" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.7142857142857" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.5714285714286" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.71428571428571" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.8571428571429" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9.14285714285714" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:14">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10">
+        <f>SUM(M3:M2225)</f>
+        <v>648100</v>
+      </c>
+    </row>
+    <row r="2" spans="10:14">
+      <c r="J2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="10:14">
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="11">
+        <v>44254</v>
+      </c>
+      <c r="M3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="10:14">
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="11">
+        <v>44254</v>
+      </c>
+      <c r="M4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="10:14">
+      <c r="J5" s="2">
+        <v>3</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="11">
+        <v>44255</v>
+      </c>
+      <c r="M5" s="2">
+        <v>190000</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="10:14">
+      <c r="J6" s="2">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="11">
+        <v>44256</v>
+      </c>
+      <c r="M6" s="2">
+        <v>150000</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="10:14">
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="11">
+        <v>44264</v>
+      </c>
+      <c r="M7" s="2">
+        <v>198100</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="12:12">
+      <c r="L8" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data till 1jun 8AM
</commit_message>
<xml_diff>
--- a/Inventory Order Book.xlsx
+++ b/Inventory Order Book.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>S.No.</t>
   </si>
@@ -157,10 +157,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="25">
@@ -194,6 +194,49 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -202,45 +245,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,13 +276,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -294,7 +301,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,13 +309,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,13 +394,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,7 +520,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,151 +544,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,6 +585,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -636,15 +645,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -690,15 +690,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -708,130 +708,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1194,13 +1194,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="6.28571428571429" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.57142857142857" style="1" customWidth="1"/>
@@ -1331,15 +1331,41 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="11">
+        <v>44289</v>
+      </c>
       <c r="E7" s="1">
         <v>10000</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>27000641</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1351,13 +1377,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.28571428571429" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.4285714285714" style="1" customWidth="1"/>
@@ -1380,7 +1406,7 @@
       </c>
       <c r="C1" s="3">
         <f>N1-G1</f>
-        <v>-79926</v>
+        <v>66847</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -1405,7 +1431,7 @@
       <c r="M1" s="9"/>
       <c r="N1" s="10">
         <f>SUM(M3:M2225)</f>
-        <v>787100</v>
+        <v>933873</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1651,6 +1677,34 @@
         <v>139000</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="10:14">
+      <c r="J9" s="1">
+        <v>7</v>
+      </c>
+      <c r="L9" s="8">
+        <v>44338</v>
+      </c>
+      <c r="M9" s="1">
+        <v>75000</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="10:14">
+      <c r="J10" s="1">
+        <v>8</v>
+      </c>
+      <c r="L10" s="8">
+        <v>44342</v>
+      </c>
+      <c r="M10" s="1">
+        <v>71773</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>